<commit_message>
compress it to exe
</commit_message>
<xml_diff>
--- a/update_market_prices.xlsx
+++ b/update_market_prices.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>证券代码</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -31,10 +31,6 @@
   </si>
   <si>
     <t>成交均价</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中科联众</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,7 +425,7 @@
   <dimension ref="A1:D160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -454,12 +450,6 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="2">
         <v>42276</v>
       </c>
@@ -468,12 +458,6 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="2">
         <v>42277</v>
       </c>
@@ -482,12 +466,6 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" s="2">
         <v>42278</v>
       </c>
@@ -496,12 +474,6 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" s="2">
         <v>42279</v>
       </c>
@@ -510,12 +482,6 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C6" s="2">
         <v>42280</v>
       </c>
@@ -524,12 +490,6 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" s="2">
         <v>42281</v>
       </c>
@@ -538,12 +498,6 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C8" s="2">
         <v>42282</v>
       </c>
@@ -552,12 +506,6 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C9" s="2">
         <v>42283</v>
       </c>
@@ -566,12 +514,6 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C10" s="2">
         <v>42284</v>
       </c>
@@ -580,12 +522,6 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C11" s="2">
         <v>42285</v>
       </c>
@@ -594,12 +530,6 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C12" s="2">
         <v>42286</v>
       </c>
@@ -608,12 +538,6 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C13" s="2">
         <v>42287</v>
       </c>
@@ -622,12 +546,6 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C14" s="2">
         <v>42288</v>
       </c>
@@ -636,12 +554,6 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C15" s="2">
         <v>42289</v>
       </c>
@@ -650,12 +562,6 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C16" s="2">
         <v>42290</v>
       </c>
@@ -663,13 +569,7 @@
         <v>4.4790999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="17" spans="3:4">
       <c r="C17" s="2">
         <v>42291</v>
       </c>
@@ -677,13 +577,7 @@
         <v>4.6690624999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="18" spans="3:4">
       <c r="C18" s="2">
         <v>42292</v>
       </c>
@@ -691,13 +585,7 @@
         <v>4.5175510204081633</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="19" spans="3:4">
       <c r="C19" s="2">
         <v>42293</v>
       </c>
@@ -705,13 +593,7 @@
         <v>4.4470689655172411</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="20" spans="3:4">
       <c r="C20" s="2">
         <v>42294</v>
       </c>
@@ -719,13 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="21" spans="3:4">
       <c r="C21" s="2">
         <v>42295</v>
       </c>
@@ -733,13 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="22" spans="3:4">
       <c r="C22" s="2">
         <v>42296</v>
       </c>
@@ -747,13 +617,7 @@
         <v>4.5312121212121212</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="23" spans="3:4">
       <c r="C23" s="2">
         <v>42297</v>
       </c>
@@ -761,13 +625,7 @@
         <v>4.4145098039215682</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="24" spans="3:4">
       <c r="C24" s="2">
         <v>42298</v>
       </c>
@@ -775,13 +633,7 @@
         <v>4.2984269662921344</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="25" spans="3:4">
       <c r="C25" s="2">
         <v>42299</v>
       </c>
@@ -789,13 +641,7 @@
         <v>4.1838461538461535</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="26" spans="3:4">
       <c r="C26" s="2">
         <v>42300</v>
       </c>
@@ -803,13 +649,7 @@
         <v>4.1497872340425532</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="27" spans="3:4">
       <c r="C27" s="2">
         <v>42301</v>
       </c>
@@ -817,13 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="28" spans="3:4">
       <c r="C28" s="2">
         <v>42302</v>
       </c>
@@ -831,13 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="29" spans="3:4">
       <c r="C29" s="2">
         <v>42303</v>
       </c>
@@ -845,13 +673,7 @@
         <v>4.1314754098360655</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="30" spans="3:4">
       <c r="C30" s="2">
         <v>42304</v>
       </c>
@@ -859,13 +681,7 @@
         <v>4.1203571428571433</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="31" spans="3:4">
       <c r="C31" s="2">
         <v>42305</v>
       </c>
@@ -873,13 +689,7 @@
         <v>4.0975409836065575</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="32" spans="3:4">
       <c r="C32" s="2">
         <v>42306</v>
       </c>
@@ -887,13 +697,7 @@
         <v>4.1334999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="33" spans="3:4">
       <c r="C33" s="2">
         <v>42307</v>
       </c>
@@ -901,13 +705,7 @@
         <v>4.1904166666666667</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="34" spans="3:4">
       <c r="C34" s="2">
         <v>42308</v>
       </c>
@@ -915,13 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="35" spans="3:4">
       <c r="C35" s="2">
         <v>42309</v>
       </c>
@@ -929,13 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="36" spans="3:4">
       <c r="C36" s="2">
         <v>42310</v>
       </c>
@@ -943,13 +729,7 @@
         <v>4.1340000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="37" spans="3:4">
       <c r="C37" s="2">
         <v>42311</v>
       </c>
@@ -957,13 +737,7 @@
         <v>4.246511627906977</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="38" spans="3:4">
       <c r="C38" s="2">
         <v>42312</v>
       </c>
@@ -971,13 +745,7 @@
         <v>4.3988333333333332</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="39" spans="3:4">
       <c r="C39" s="2">
         <v>42313</v>
       </c>
@@ -985,13 +753,7 @@
         <v>4.5090714285714286</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="40" spans="3:4">
       <c r="C40" s="2">
         <v>42314</v>
       </c>
@@ -999,13 +761,7 @@
         <v>4.4306435643564352</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="41" spans="3:4">
       <c r="C41" s="2">
         <v>42315</v>
       </c>
@@ -1013,13 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="42" spans="3:4">
       <c r="C42" s="2">
         <v>42316</v>
       </c>
@@ -1027,13 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="43" spans="3:4">
       <c r="C43" s="2">
         <v>42317</v>
       </c>
@@ -1041,13 +785,7 @@
         <v>4.4315384615384614</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="44" spans="3:4">
       <c r="C44" s="2">
         <v>42318</v>
       </c>
@@ -1055,13 +793,7 @@
         <v>4.4783333333333335</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="45" spans="3:4">
       <c r="C45" s="2">
         <v>42319</v>
       </c>
@@ -1069,13 +801,7 @@
         <v>4.4823809523809528</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="46" spans="3:4">
       <c r="C46" s="2">
         <v>42320</v>
       </c>
@@ -1083,13 +809,7 @@
         <v>4.5231250000000003</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="47" spans="3:4">
       <c r="C47" s="2">
         <v>42321</v>
       </c>
@@ -1097,13 +817,7 @@
         <v>4.5703076923076926</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="48" spans="3:4">
       <c r="C48" s="2">
         <v>42322</v>
       </c>
@@ -1111,13 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="49" spans="3:4">
       <c r="C49" s="2">
         <v>42323</v>
       </c>
@@ -1125,13 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="50" spans="3:4">
       <c r="C50" s="2">
         <v>42324</v>
       </c>
@@ -1139,13 +841,7 @@
         <v>4.6255038759689926</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="51" spans="3:4">
       <c r="C51" s="2">
         <v>42325</v>
       </c>
@@ -1153,13 +849,7 @@
         <v>4.9318348623853208</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="52" spans="3:4">
       <c r="C52" s="2">
         <v>42326</v>
       </c>
@@ -1167,13 +857,7 @@
         <v>4.9860447761194031</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="53" spans="3:4">
       <c r="C53" s="2">
         <v>42327</v>
       </c>
@@ -1181,13 +865,7 @@
         <v>4.9434883720930234</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="54" spans="3:4">
       <c r="C54" s="2">
         <v>42328</v>
       </c>
@@ -1195,13 +873,7 @@
         <v>4.987333333333333</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="55" spans="3:4">
       <c r="C55" s="2">
         <v>42329</v>
       </c>
@@ -1209,13 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="56" spans="3:4">
       <c r="C56" s="2">
         <v>42330</v>
       </c>
@@ -1223,13 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="57" spans="3:4">
       <c r="C57" s="2">
         <v>42331</v>
       </c>
@@ -1237,13 +897,7 @@
         <v>5.2469415807560136</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="58" spans="3:4">
       <c r="C58" s="2">
         <v>42332</v>
       </c>
@@ -1251,13 +905,7 @@
         <v>5.1582692307692311</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="59" spans="3:4">
       <c r="C59" s="2">
         <v>42333</v>
       </c>
@@ -1265,13 +913,7 @@
         <v>5.2267415730337081</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="60" spans="3:4">
       <c r="C60" s="2">
         <v>42334</v>
       </c>
@@ -1279,13 +921,7 @@
         <v>5.1879268292682923</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="61" spans="3:4">
       <c r="C61" s="2">
         <v>42335</v>
       </c>
@@ -1293,13 +929,7 @@
         <v>5.07328125</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="62" spans="3:4">
       <c r="C62" s="2">
         <v>42336</v>
       </c>
@@ -1307,13 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="63" spans="3:4">
       <c r="C63" s="2">
         <v>42337</v>
       </c>
@@ -1321,13 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="64" spans="3:4">
       <c r="C64" s="2">
         <v>42338</v>
       </c>
@@ -1335,13 +953,7 @@
         <v>5.2091095890410957</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="65" spans="3:4">
       <c r="C65" s="2">
         <v>42339</v>
       </c>
@@ -1349,13 +961,7 @@
         <v>5.1085714285714285</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="66" spans="3:4">
       <c r="C66" s="2">
         <v>42340</v>
       </c>
@@ -1363,13 +969,7 @@
         <v>5.1230000000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="67" spans="3:4">
       <c r="C67" s="2">
         <v>42341</v>
       </c>
@@ -1377,13 +977,7 @@
         <v>4.9940983606557374</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="68" spans="3:4">
       <c r="C68" s="2">
         <v>42342</v>
       </c>
@@ -1391,13 +985,7 @@
         <v>4.8738495575221235</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="69" spans="3:4">
       <c r="C69" s="2">
         <v>42343</v>
       </c>
@@ -1405,13 +993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="70" spans="3:4">
       <c r="C70" s="2">
         <v>42344</v>
       </c>
@@ -1419,13 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="71" spans="3:4">
       <c r="C71" s="2">
         <v>42345</v>
       </c>
@@ -1433,13 +1009,7 @@
         <v>4.8970000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="72" spans="3:4">
       <c r="C72" s="2">
         <v>42346</v>
       </c>
@@ -1447,13 +1017,7 @@
         <v>4.996279069767442</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="73" spans="3:4">
       <c r="C73" s="2">
         <v>42347</v>
       </c>
@@ -1461,13 +1025,7 @@
         <v>5.0253125000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="74" spans="3:4">
       <c r="C74" s="2">
         <v>42348</v>
       </c>
@@ -1475,13 +1033,7 @@
         <v>5.0056074766355136</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="75" spans="3:4">
       <c r="C75" s="2">
         <v>42349</v>
       </c>
@@ -1489,13 +1041,7 @@
         <v>5.0276923076923081</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="76" spans="3:4">
       <c r="C76" s="2">
         <v>42350</v>
       </c>
@@ -1503,13 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="77" spans="3:4">
       <c r="C77" s="2">
         <v>42351</v>
       </c>
@@ -1517,13 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="78" spans="3:4">
       <c r="C78" s="2">
         <v>42352</v>
       </c>
@@ -1531,13 +1065,7 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="79" spans="3:4">
       <c r="C79" s="2">
         <v>42353</v>
       </c>
@@ -1545,13 +1073,7 @@
         <v>4.9521739130434783</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="80" spans="3:4">
       <c r="C80" s="2">
         <v>42354</v>
       </c>
@@ -1559,13 +1081,7 @@
         <v>4.9064444444444444</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="81" spans="3:4">
       <c r="C81" s="2">
         <v>42355</v>
       </c>
@@ -1573,13 +1089,7 @@
         <v>4.8886075949367092</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="82" spans="3:4">
       <c r="C82" s="2">
         <v>42356</v>
       </c>
@@ -1587,13 +1097,7 @@
         <v>4.9756410256410257</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="83" spans="3:4">
       <c r="C83" s="2">
         <v>42357</v>
       </c>
@@ -1601,13 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="84" spans="3:4">
       <c r="C84" s="2">
         <v>42358</v>
       </c>
@@ -1615,13 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="85" spans="3:4">
       <c r="C85" s="2">
         <v>42359</v>
       </c>
@@ -1629,13 +1121,7 @@
         <v>5.0298412698412696</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="86" spans="3:4">
       <c r="C86" s="2">
         <v>42360</v>
       </c>
@@ -1643,13 +1129,7 @@
         <v>4.8468421052631578</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="87" spans="3:4">
       <c r="C87" s="2">
         <v>42361</v>
       </c>
@@ -1657,13 +1137,7 @@
         <v>4.8277310924369745</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="88" spans="3:4">
       <c r="C88" s="2">
         <v>42362</v>
       </c>
@@ -1671,13 +1145,7 @@
         <v>4.6689502762430939</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="89" spans="3:4">
       <c r="C89" s="2">
         <v>42363</v>
       </c>
@@ -1685,13 +1153,7 @@
         <v>4.8587037037037035</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="90" spans="3:4">
       <c r="C90" s="2">
         <v>42364</v>
       </c>
@@ -1699,13 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="91" spans="3:4">
       <c r="C91" s="2">
         <v>42365</v>
       </c>
@@ -1713,13 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="92" spans="3:4">
       <c r="C92" s="2">
         <v>42366</v>
       </c>
@@ -1727,13 +1177,7 @@
         <v>4.8469639769960837</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="93" spans="3:4">
       <c r="C93" s="2">
         <v>42367</v>
       </c>
@@ -1741,13 +1185,7 @@
         <v>5.025675675675676</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="94" spans="3:4">
       <c r="C94" s="2">
         <v>42368</v>
       </c>
@@ -1755,13 +1193,7 @@
         <v>4.9940909090909091</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="95" spans="3:4">
       <c r="C95" s="2">
         <v>42369</v>
       </c>
@@ -1769,13 +1201,7 @@
         <v>5.093877551020408</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="96" spans="3:4">
       <c r="C96" s="2">
         <v>42370</v>
       </c>
@@ -1783,13 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="97" spans="3:4">
       <c r="C97" s="2">
         <v>42371</v>
       </c>
@@ -1797,13 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="98" spans="3:4">
       <c r="C98" s="2">
         <v>42372</v>
       </c>
@@ -1811,13 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="99" spans="3:4">
       <c r="C99" s="2">
         <v>42373</v>
       </c>
@@ -1825,13 +1233,7 @@
         <v>5.0229824561403511</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="100" spans="3:4">
       <c r="C100" s="2">
         <v>42374</v>
       </c>
@@ -1839,13 +1241,7 @@
         <v>4.9012643678160916</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="101" spans="3:4">
       <c r="C101" s="2">
         <v>42375</v>
       </c>
@@ -1853,13 +1249,7 @@
         <v>4.9649999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="102" spans="3:4">
       <c r="C102" s="2">
         <v>42376</v>
       </c>
@@ -1867,13 +1257,7 @@
         <v>4.6403610108303246</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="103" spans="3:4">
       <c r="C103" s="2">
         <v>42377</v>
       </c>
@@ -1881,13 +1265,7 @@
         <v>4.7445833333333329</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="104" spans="3:4">
       <c r="C104" s="2">
         <v>42378</v>
       </c>
@@ -1895,13 +1273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="105" spans="3:4">
       <c r="C105" s="2">
         <v>42379</v>
       </c>
@@ -1909,13 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="106" spans="3:4">
       <c r="C106" s="2">
         <v>42380</v>
       </c>
@@ -1923,13 +1289,7 @@
         <v>4.5846808510638297</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="107" spans="3:4">
       <c r="C107" s="2">
         <v>42381</v>
       </c>
@@ -1937,13 +1297,7 @@
         <v>4.3961111111111109</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="108" spans="3:4">
       <c r="C108" s="2">
         <v>42382</v>
       </c>
@@ -1951,13 +1305,7 @@
         <v>4.276071428571429</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="109" spans="3:4">
       <c r="C109" s="2">
         <v>42383</v>
       </c>
@@ -1965,13 +1313,7 @@
         <v>4.4782142857142855</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="110" spans="3:4">
       <c r="C110" s="2">
         <v>42384</v>
       </c>
@@ -1979,13 +1321,7 @@
         <v>4.8017796610169494</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="111" spans="3:4">
       <c r="C111" s="2">
         <v>42385</v>
       </c>
@@ -1993,13 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="112" spans="3:4">
       <c r="C112" s="2">
         <v>42386</v>
       </c>
@@ -2007,13 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="113" spans="3:4">
       <c r="C113" s="2">
         <v>42387</v>
       </c>
@@ -2021,13 +1345,7 @@
         <v>4.6864705882352942</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="114" spans="3:4">
       <c r="C114" s="2">
         <v>42388</v>
       </c>
@@ -2035,13 +1353,7 @@
         <v>4.7027272727272731</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="115" spans="3:4">
       <c r="C115" s="2">
         <v>42389</v>
       </c>
@@ -2049,13 +1361,7 @@
         <v>4.8681065088757398</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="116" spans="3:4">
       <c r="C116" s="2">
         <v>42390</v>
       </c>
@@ -2063,13 +1369,7 @@
         <v>4.8813235294117643</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="117" spans="3:4">
       <c r="C117" s="2">
         <v>42391</v>
       </c>
@@ -2077,13 +1377,7 @@
         <v>4.9807377630645542</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="118" spans="3:4">
       <c r="C118" s="2">
         <v>42392</v>
       </c>
@@ -2091,13 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="119" spans="3:4">
       <c r="C119" s="2">
         <v>42393</v>
       </c>
@@ -2105,13 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="1">
-        <v>430083</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="120" spans="3:4">
       <c r="C120" s="2">
         <v>42394</v>
       </c>
@@ -2119,28 +1401,28 @@
         <v>5.1336915887850472</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="3:4">
       <c r="C121" s="2"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="3:4">
       <c r="C122" s="2"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="3:4">
       <c r="C123" s="2"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="3:4">
       <c r="C124" s="2"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="3:4">
       <c r="C125" s="2"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="3:4">
       <c r="C126" s="2"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="3:4">
       <c r="C127" s="2"/>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="3:4">
       <c r="C128" s="2"/>
     </row>
     <row r="129" spans="3:3">

</xml_diff>